<commit_message>
Uploading Canadian Census Files
</commit_message>
<xml_diff>
--- a/US_Population_Data/US_Population_Data_Summary.xlsx
+++ b/US_Population_Data/US_Population_Data_Summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122BD7BB-6E7E-4F2D-A784-AF02703E199B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A9C9D8-4424-4FEF-82AF-D4CBE5A4A10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1802,11 +1802,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -2210,16 +2210,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -2229,400 +2229,400 @@
       <c r="C3" s="16"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="14"/>
     </row>
     <row r="6" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="14"/>
     </row>
     <row r="13" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="14"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
     </row>
     <row r="15" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="14"/>
     </row>
     <row r="16" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="14"/>
     </row>
     <row r="17" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
     </row>
     <row r="19" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
     </row>
     <row r="21" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="14"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
     </row>
     <row r="25" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="14"/>
     </row>
     <row r="26" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="15"/>
+      <c r="C26" s="14"/>
     </row>
     <row r="27" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="14"/>
     </row>
     <row r="28" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="14"/>
     </row>
     <row r="29" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="14"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
     </row>
     <row r="31" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="14"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
     </row>
     <row r="33" spans="1:3" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="15"/>
+      <c r="C33" s="14"/>
     </row>
     <row r="34" spans="1:3" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="15"/>
+      <c r="C34" s="14"/>
     </row>
     <row r="35" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" spans="1:3" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="15"/>
+      <c r="C36" s="14"/>
     </row>
     <row r="37" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="15"/>
+      <c r="C37" s="14"/>
     </row>
     <row r="38" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="15"/>
+      <c r="C38" s="14"/>
     </row>
     <row r="39" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="15"/>
+      <c r="C39" s="14"/>
     </row>
     <row r="40" spans="1:3" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="15"/>
+      <c r="C40" s="14"/>
     </row>
     <row r="41" spans="1:3" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="15"/>
+      <c r="C41" s="14"/>
     </row>
     <row r="42" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="15"/>
+      <c r="C42" s="14"/>
     </row>
     <row r="43" spans="1:3" ht="176.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="15"/>
+      <c r="C43" s="14"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
     </row>
     <row r="45" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="15"/>
+      <c r="C45" s="14"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating final presentation to branch
</commit_message>
<xml_diff>
--- a/US_Population_Data/US_Population_Data_Summary.xlsx
+++ b/US_Population_Data/US_Population_Data_Summary.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD50C82-2783-43F8-8AB4-373B4FBF2D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91368090-9112-4E5D-96D0-419E01DA3638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -752,7 +752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B7F75B-4B10-4D08-90CC-6F4C637B5C45}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>